<commit_message>
Enhanced layout of leader board and score board
</commit_message>
<xml_diff>
--- a/scoreboard.xlsx
+++ b/scoreboard.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="8">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="11">
   <si>
     <t>KAUSAR</t>
   </si>
@@ -31,13 +31,22 @@
     <t>SHAQUIB</t>
   </si>
   <si>
-    <t>-5</t>
+    <t>a</t>
   </si>
   <si>
-    <t>-6</t>
+    <t>B</t>
   </si>
   <si>
-    <t>11</t>
+    <t>c</t>
+  </si>
+  <si>
+    <t>d</t>
+  </si>
+  <si>
+    <t>e</t>
+  </si>
+  <si>
+    <t>-1</t>
   </si>
 </sst>
 </file>
@@ -395,13 +404,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:E26"/>
+  <dimension ref="A1:J62"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:5">
+    <row r="1" spans="1:10">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -417,8 +426,23 @@
       <c r="E1" s="1" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="2" spans="1:5">
+      <c r="F1" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="I1" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="J1" s="1" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="2" spans="1:10">
       <c r="A2">
         <v>-5</v>
       </c>
@@ -432,7 +456,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="3" spans="1:5">
+    <row r="3" spans="1:10">
       <c r="C3">
         <v>-3</v>
       </c>
@@ -443,7 +467,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="4" spans="1:5">
+    <row r="4" spans="1:10">
       <c r="C4">
         <v>-5</v>
       </c>
@@ -454,7 +478,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="5" spans="1:5">
+    <row r="5" spans="1:10">
       <c r="C5">
         <v>0</v>
       </c>
@@ -465,7 +489,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:5">
+    <row r="6" spans="1:10">
       <c r="C6">
         <v>-5</v>
       </c>
@@ -476,7 +500,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="7" spans="1:5">
+    <row r="7" spans="1:10">
       <c r="C7">
         <v>-5</v>
       </c>
@@ -487,7 +511,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="8" spans="1:5">
+    <row r="8" spans="1:10">
       <c r="C8">
         <v>-5</v>
       </c>
@@ -498,7 +522,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="9" spans="1:5">
+    <row r="9" spans="1:10">
       <c r="C9">
         <v>-2</v>
       </c>
@@ -509,7 +533,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="10" spans="1:5">
+    <row r="10" spans="1:10">
       <c r="C10">
         <v>-6</v>
       </c>
@@ -520,7 +544,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="11" spans="1:5">
+    <row r="11" spans="1:10">
       <c r="C11">
         <v>-5</v>
       </c>
@@ -528,7 +552,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="12" spans="1:5">
+    <row r="12" spans="1:10">
       <c r="C12">
         <v>-2</v>
       </c>
@@ -536,7 +560,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="13" spans="1:5">
+    <row r="13" spans="1:10">
       <c r="B13">
         <v>-6</v>
       </c>
@@ -550,7 +574,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="14" spans="1:5">
+    <row r="14" spans="1:10">
       <c r="B14">
         <v>-7</v>
       </c>
@@ -564,7 +588,7 @@
         <v>-15</v>
       </c>
     </row>
-    <row r="15" spans="1:5">
+    <row r="15" spans="1:10">
       <c r="B15">
         <v>0</v>
       </c>
@@ -578,7 +602,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="16" spans="1:5">
+    <row r="16" spans="1:10">
       <c r="B16">
         <v>0</v>
       </c>
@@ -592,7 +616,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="17" spans="2:5">
+    <row r="17" spans="2:8">
       <c r="B17">
         <v>0</v>
       </c>
@@ -606,7 +630,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="18" spans="2:5">
+    <row r="18" spans="2:8">
       <c r="B18">
         <v>0</v>
       </c>
@@ -620,7 +644,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="19" spans="2:5">
+    <row r="19" spans="2:8">
       <c r="B19">
         <v>0</v>
       </c>
@@ -634,7 +658,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="20" spans="2:5">
+    <row r="20" spans="2:8">
       <c r="B20">
         <v>0</v>
       </c>
@@ -648,7 +672,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="21" spans="2:5">
+    <row r="21" spans="2:8">
       <c r="B21">
         <v>0</v>
       </c>
@@ -662,7 +686,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="22" spans="2:5">
+    <row r="22" spans="2:8">
       <c r="B22">
         <v>0</v>
       </c>
@@ -676,7 +700,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="23" spans="2:5">
+    <row r="23" spans="2:8">
       <c r="B23">
         <v>-12</v>
       </c>
@@ -687,7 +711,7 @@
         <v>-23</v>
       </c>
     </row>
-    <row r="24" spans="2:5">
+    <row r="24" spans="2:8">
       <c r="B24">
         <v>0</v>
       </c>
@@ -698,7 +722,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="25" spans="2:5">
+    <row r="25" spans="2:8">
       <c r="B25">
         <v>-5</v>
       </c>
@@ -709,15 +733,486 @@
         <v>11</v>
       </c>
     </row>
-    <row r="26" spans="2:5">
-      <c r="C26" t="s">
-        <v>5</v>
-      </c>
-      <c r="D26" t="s">
+    <row r="26" spans="2:8">
+      <c r="C26">
+        <v>-5</v>
+      </c>
+      <c r="D26">
+        <v>-6</v>
+      </c>
+      <c r="E26">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="27" spans="2:8">
+      <c r="C27">
+        <v>-5</v>
+      </c>
+      <c r="D27">
+        <v>-6</v>
+      </c>
+      <c r="E27">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="28" spans="2:8">
+      <c r="C28">
+        <v>-5</v>
+      </c>
+      <c r="D28">
+        <v>-3</v>
+      </c>
+      <c r="E28">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="29" spans="2:8">
+      <c r="C29">
+        <v>-5</v>
+      </c>
+      <c r="D29">
+        <v>-3</v>
+      </c>
+      <c r="E29">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="30" spans="2:8">
+      <c r="C30">
+        <v>-6</v>
+      </c>
+      <c r="D30">
+        <v>-3</v>
+      </c>
+      <c r="E30">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="31" spans="2:8">
+      <c r="C31">
+        <v>0</v>
+      </c>
+      <c r="D31">
+        <v>0</v>
+      </c>
+      <c r="E31">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="32" spans="2:8">
+      <c r="F32">
+        <v>-5</v>
+      </c>
+      <c r="G32">
+        <v>-6</v>
+      </c>
+      <c r="H32">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="33" spans="6:10">
+      <c r="F33">
+        <v>0</v>
+      </c>
+      <c r="G33">
+        <v>0</v>
+      </c>
+      <c r="H33">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="34" spans="6:10">
+      <c r="F34">
+        <v>-5</v>
+      </c>
+      <c r="G34">
+        <v>-6</v>
+      </c>
+      <c r="H34">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="35" spans="6:10">
+      <c r="F35">
+        <v>-5</v>
+      </c>
+      <c r="G35">
+        <v>-6</v>
+      </c>
+      <c r="H35">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="36" spans="6:10">
+      <c r="F36">
+        <v>-5</v>
+      </c>
+      <c r="G36">
+        <v>-3</v>
+      </c>
+      <c r="H36">
+        <v>-2</v>
+      </c>
+    </row>
+    <row r="37" spans="6:10">
+      <c r="F37">
+        <v>-5</v>
+      </c>
+      <c r="G37">
+        <v>-6</v>
+      </c>
+      <c r="H37">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="38" spans="6:10">
+      <c r="F38">
+        <v>-6</v>
+      </c>
+      <c r="G38">
+        <v>-3</v>
+      </c>
+      <c r="H38">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="39" spans="6:10">
+      <c r="F39">
+        <v>-5</v>
+      </c>
+      <c r="G39">
+        <v>-3</v>
+      </c>
+      <c r="H39">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="40" spans="6:10">
+      <c r="F40">
+        <v>-5</v>
+      </c>
+      <c r="G40">
+        <v>-6</v>
+      </c>
+      <c r="H40">
+        <v>-3</v>
+      </c>
+    </row>
+    <row r="41" spans="6:10">
+      <c r="F41">
+        <v>0</v>
+      </c>
+      <c r="G41">
+        <v>0</v>
+      </c>
+      <c r="H41">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="42" spans="6:10">
+      <c r="F42">
+        <v>-6</v>
+      </c>
+      <c r="G42">
+        <v>-3</v>
+      </c>
+      <c r="H42">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="43" spans="6:10">
+      <c r="F43">
+        <v>-6</v>
+      </c>
+      <c r="G43">
+        <v>-5</v>
+      </c>
+      <c r="H43">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="44" spans="6:10">
+      <c r="F44">
+        <v>-5</v>
+      </c>
+      <c r="G44">
+        <v>-3</v>
+      </c>
+      <c r="H44">
+        <v>-3</v>
+      </c>
+    </row>
+    <row r="45" spans="6:10">
+      <c r="F45">
+        <v>-5</v>
+      </c>
+      <c r="G45">
+        <v>-6</v>
+      </c>
+      <c r="H45">
+        <v>-3</v>
+      </c>
+      <c r="I45">
+        <v>-3</v>
+      </c>
+      <c r="J45">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="46" spans="6:10">
+      <c r="F46">
+        <v>0</v>
+      </c>
+      <c r="G46">
+        <v>0</v>
+      </c>
+      <c r="H46">
+        <v>0</v>
+      </c>
+      <c r="I46">
+        <v>0</v>
+      </c>
+      <c r="J46">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="47" spans="6:10">
+      <c r="F47">
+        <v>0</v>
+      </c>
+      <c r="G47">
+        <v>0</v>
+      </c>
+      <c r="H47">
+        <v>0</v>
+      </c>
+      <c r="I47">
+        <v>0</v>
+      </c>
+      <c r="J47">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="48" spans="6:10">
+      <c r="F48">
+        <v>0</v>
+      </c>
+      <c r="G48">
+        <v>0</v>
+      </c>
+      <c r="H48">
+        <v>0</v>
+      </c>
+      <c r="I48">
+        <v>0</v>
+      </c>
+      <c r="J48">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="49" spans="1:10">
+      <c r="F49">
+        <v>-6</v>
+      </c>
+      <c r="G49">
+        <v>-3</v>
+      </c>
+      <c r="H49">
+        <v>-3</v>
+      </c>
+      <c r="I49">
+        <v>-3</v>
+      </c>
+      <c r="J49">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="50" spans="1:10">
+      <c r="F50">
+        <v>0</v>
+      </c>
+      <c r="G50">
+        <v>0</v>
+      </c>
+      <c r="H50">
+        <v>0</v>
+      </c>
+      <c r="I50">
+        <v>0</v>
+      </c>
+      <c r="J50">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="51" spans="1:10">
+      <c r="F51">
+        <v>-5</v>
+      </c>
+      <c r="G51">
+        <v>-3</v>
+      </c>
+      <c r="H51">
+        <v>8</v>
+      </c>
+      <c r="I51">
+        <v>8</v>
+      </c>
+      <c r="J51">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="52" spans="1:10">
+      <c r="F52">
+        <v>0</v>
+      </c>
+      <c r="G52">
+        <v>0</v>
+      </c>
+      <c r="H52">
+        <v>0</v>
+      </c>
+      <c r="I52">
+        <v>0</v>
+      </c>
+      <c r="J52">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="53" spans="1:10">
+      <c r="F53">
+        <v>0</v>
+      </c>
+      <c r="G53">
+        <v>0</v>
+      </c>
+      <c r="H53">
+        <v>0</v>
+      </c>
+      <c r="I53">
+        <v>0</v>
+      </c>
+      <c r="J53">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="54" spans="1:10">
+      <c r="F54">
+        <v>0</v>
+      </c>
+      <c r="G54">
+        <v>0</v>
+      </c>
+      <c r="H54">
+        <v>0</v>
+      </c>
+      <c r="I54">
+        <v>0</v>
+      </c>
+      <c r="J54">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="55" spans="1:10">
+      <c r="F55">
+        <v>-5</v>
+      </c>
+      <c r="G55">
+        <v>-3</v>
+      </c>
+      <c r="H55">
+        <v>-3</v>
+      </c>
+      <c r="I55">
+        <v>-2</v>
+      </c>
+      <c r="J55">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="56" spans="1:10">
+      <c r="C56">
+        <v>-5</v>
+      </c>
+      <c r="D56">
+        <v>-6</v>
+      </c>
+    </row>
+    <row r="57" spans="1:10">
+      <c r="C57">
+        <v>-6</v>
+      </c>
+      <c r="D57">
         <v>6</v>
       </c>
-      <c r="E26" t="s">
-        <v>7</v>
+    </row>
+    <row r="58" spans="1:10">
+      <c r="A58">
+        <v>-5</v>
+      </c>
+      <c r="C58">
+        <v>-3</v>
+      </c>
+      <c r="D58">
+        <v>-2</v>
+      </c>
+      <c r="E58">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="59" spans="1:10">
+      <c r="A59">
+        <v>18</v>
+      </c>
+      <c r="C59">
+        <v>-9</v>
+      </c>
+      <c r="D59">
+        <v>-6</v>
+      </c>
+      <c r="E59">
+        <v>-3</v>
+      </c>
+    </row>
+    <row r="60" spans="1:10">
+      <c r="A60">
+        <v>-10</v>
+      </c>
+      <c r="C60">
+        <v>-10</v>
+      </c>
+      <c r="D60">
+        <v>-10</v>
+      </c>
+      <c r="E60">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="61" spans="1:10">
+      <c r="A61">
+        <v>0</v>
+      </c>
+      <c r="C61">
+        <v>0</v>
+      </c>
+      <c r="D61">
+        <v>0</v>
+      </c>
+      <c r="E61">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="62" spans="1:10">
+      <c r="A62" t="s">
+        <v>10</v>
+      </c>
+      <c r="C62" t="s">
+        <v>10</v>
+      </c>
+      <c r="D62" t="s">
+        <v>10</v>
+      </c>
+      <c r="E62" t="s">
+        <v>10</v>
       </c>
     </row>
   </sheetData>

</xml_diff>